<commit_message>
Replace CEM by CB in Excel in March 2023 data
</commit_message>
<xml_diff>
--- a/3 TP Analysis/01 - Data/PROCESSED_benthic_cover_March_2023.xlsx
+++ b/3 TP Analysis/01 - Data/PROCESSED_benthic_cover_March_2023.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Shannon/GitHub/NFI_benthic_community/3 TP Analysis/01 - Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DB27DB-286E-A242-BF47-0739402D72A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62F06A4C-2438-A846-869B-DCC5ED918125}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="900" yWindow="500" windowWidth="27900" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,156 +113,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>March_2023CEM4_10.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_1.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_2.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_3.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_4.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_5.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_6.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_7.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_8.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM4_9.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_10.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_1.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_2.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_3.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_4.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_5.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_6.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_7.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_8.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM5_9.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_10.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_1.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_2.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_3.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_4.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_5.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_6.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_7.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_8.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM6_9.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_10.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_1.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_2.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_3.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_4.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_5.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_6.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_7.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_8.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM7_9.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_10.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_1.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_2.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_3.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_4.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_5.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_6.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_7.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_8.JPG</t>
-  </si>
-  <si>
-    <t>March_2023CEM8_9.JPG</t>
-  </si>
-  <si>
     <t>March_2023EB10_10.JPG</t>
   </si>
   <si>
@@ -1428,6 +1278,156 @@
   </si>
   <si>
     <t>Image_ID</t>
+  </si>
+  <si>
+    <t>March_2023CB4_10.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_1.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_2.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_3.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_4.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_5.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_6.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_7.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_8.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB4_9.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_10.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_1.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_2.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_3.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_4.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_5.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_6.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_7.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_8.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB5_9.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_10.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_1.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_2.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_3.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_4.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_5.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_6.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_7.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_8.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB6_9.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_10.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_1.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_2.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_3.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_4.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_5.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_6.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_7.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_8.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB7_9.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_10.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_1.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_2.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_3.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_4.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_5.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_6.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_7.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_8.JPG</t>
+  </si>
+  <si>
+    <t>March_2023CB8_9.JPG</t>
   </si>
 </sst>
 </file>
@@ -1770,8 +1770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE431"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A390" zoomScale="125" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1782,7 +1782,7 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>468</v>
+        <v>418</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -1877,7 +1877,7 @@
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>419</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1972,7 +1972,7 @@
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>420</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>421</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2162,7 +2162,7 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>422</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>423</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2352,7 +2352,7 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>424</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2447,7 +2447,7 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>425</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2542,7 +2542,7 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>426</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2637,7 +2637,7 @@
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>38</v>
+        <v>427</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>428</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2827,7 +2827,7 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>429</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2922,7 +2922,7 @@
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>430</v>
       </c>
       <c r="B13">
         <v>7</v>
@@ -3017,7 +3017,7 @@
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>431</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>432</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -3207,7 +3207,7 @@
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>44</v>
+        <v>433</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -3302,7 +3302,7 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>434</v>
       </c>
       <c r="B17">
         <v>0</v>
@@ -3397,7 +3397,7 @@
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>435</v>
       </c>
       <c r="B18">
         <v>0</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>47</v>
+        <v>436</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3587,7 +3587,7 @@
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>437</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3682,7 +3682,7 @@
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>49</v>
+        <v>438</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -3777,7 +3777,7 @@
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>50</v>
+        <v>439</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -3872,7 +3872,7 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>440</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -3967,7 +3967,7 @@
     </row>
     <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>441</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -4062,7 +4062,7 @@
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>53</v>
+        <v>442</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4157,7 +4157,7 @@
     </row>
     <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>443</v>
       </c>
       <c r="B26">
         <v>1</v>
@@ -4252,7 +4252,7 @@
     </row>
     <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>444</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4347,7 +4347,7 @@
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>445</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>57</v>
+        <v>446</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4537,7 +4537,7 @@
     </row>
     <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>58</v>
+        <v>447</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4632,7 +4632,7 @@
     </row>
     <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>448</v>
       </c>
       <c r="B31">
         <v>0</v>
@@ -4727,7 +4727,7 @@
     </row>
     <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>449</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -4822,7 +4822,7 @@
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>450</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -4917,7 +4917,7 @@
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>451</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -5012,7 +5012,7 @@
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>452</v>
       </c>
       <c r="B35">
         <v>0</v>
@@ -5107,7 +5107,7 @@
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>453</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -5202,7 +5202,7 @@
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>454</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -5297,7 +5297,7 @@
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>455</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -5392,7 +5392,7 @@
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>456</v>
       </c>
       <c r="B39">
         <v>3</v>
@@ -5487,7 +5487,7 @@
     </row>
     <row r="40" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>457</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -5582,7 +5582,7 @@
     </row>
     <row r="41" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>458</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -5677,7 +5677,7 @@
     </row>
     <row r="42" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>459</v>
       </c>
       <c r="B42">
         <v>19</v>
@@ -5772,7 +5772,7 @@
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>460</v>
       </c>
       <c r="B43">
         <v>9</v>
@@ -5867,7 +5867,7 @@
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>461</v>
       </c>
       <c r="B44">
         <v>6</v>
@@ -5962,7 +5962,7 @@
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>462</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -6057,7 +6057,7 @@
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>463</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -6152,7 +6152,7 @@
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>464</v>
       </c>
       <c r="B47">
         <v>22</v>
@@ -6247,7 +6247,7 @@
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>465</v>
       </c>
       <c r="B48">
         <v>17</v>
@@ -6342,7 +6342,7 @@
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>466</v>
       </c>
       <c r="B49">
         <v>2</v>
@@ -6437,7 +6437,7 @@
     </row>
     <row r="50" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>467</v>
       </c>
       <c r="B50">
         <v>6</v>
@@ -6532,7 +6532,7 @@
     </row>
     <row r="51" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>468</v>
       </c>
       <c r="B51">
         <v>6</v>
@@ -6627,7 +6627,7 @@
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="B52">
         <v>2</v>
@@ -6722,7 +6722,7 @@
     </row>
     <row r="53" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -6817,7 +6817,7 @@
     </row>
     <row r="54" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6912,7 +6912,7 @@
     </row>
     <row r="55" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -7007,7 +7007,7 @@
     </row>
     <row r="56" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -7102,7 +7102,7 @@
     </row>
     <row r="57" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -7197,7 +7197,7 @@
     </row>
     <row r="58" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>86</v>
+        <v>36</v>
       </c>
       <c r="B58">
         <v>0</v>
@@ -7292,7 +7292,7 @@
     </row>
     <row r="59" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>87</v>
+        <v>37</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -7387,7 +7387,7 @@
     </row>
     <row r="60" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>88</v>
+        <v>38</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -7482,7 +7482,7 @@
     </row>
     <row r="61" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>89</v>
+        <v>39</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -7577,7 +7577,7 @@
     </row>
     <row r="62" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="B62">
         <v>0</v>
@@ -7672,7 +7672,7 @@
     </row>
     <row r="63" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>41</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -7767,7 +7767,7 @@
     </row>
     <row r="64" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -7862,7 +7862,7 @@
     </row>
     <row r="65" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="B65">
         <v>0</v>
@@ -7957,7 +7957,7 @@
     </row>
     <row r="66" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>94</v>
+        <v>44</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -8052,7 +8052,7 @@
     </row>
     <row r="67" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>95</v>
+        <v>45</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -8147,7 +8147,7 @@
     </row>
     <row r="68" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>96</v>
+        <v>46</v>
       </c>
       <c r="B68">
         <v>7</v>
@@ -8242,7 +8242,7 @@
     </row>
     <row r="69" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>97</v>
+        <v>47</v>
       </c>
       <c r="B69">
         <v>56</v>
@@ -8337,7 +8337,7 @@
     </row>
     <row r="70" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>98</v>
+        <v>48</v>
       </c>
       <c r="B70">
         <v>75</v>
@@ -8432,7 +8432,7 @@
     </row>
     <row r="71" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>99</v>
+        <v>49</v>
       </c>
       <c r="B71">
         <v>6</v>
@@ -8527,7 +8527,7 @@
     </row>
     <row r="72" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="B72">
         <v>0</v>
@@ -8622,7 +8622,7 @@
     </row>
     <row r="73" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -8717,7 +8717,7 @@
     </row>
     <row r="74" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="B74">
         <v>0</v>
@@ -8812,7 +8812,7 @@
     </row>
     <row r="75" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>103</v>
+        <v>53</v>
       </c>
       <c r="B75">
         <v>0</v>
@@ -8907,7 +8907,7 @@
     </row>
     <row r="76" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>104</v>
+        <v>54</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -9002,7 +9002,7 @@
     </row>
     <row r="77" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>105</v>
+        <v>55</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -9097,7 +9097,7 @@
     </row>
     <row r="78" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -9192,7 +9192,7 @@
     </row>
     <row r="79" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>107</v>
+        <v>57</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -9287,7 +9287,7 @@
     </row>
     <row r="80" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -9382,7 +9382,7 @@
     </row>
     <row r="81" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>109</v>
+        <v>59</v>
       </c>
       <c r="B81">
         <v>0</v>
@@ -9477,7 +9477,7 @@
     </row>
     <row r="82" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>110</v>
+        <v>60</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -9572,7 +9572,7 @@
     </row>
     <row r="83" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -9667,7 +9667,7 @@
     </row>
     <row r="84" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>112</v>
+        <v>62</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -9762,7 +9762,7 @@
     </row>
     <row r="85" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>113</v>
+        <v>63</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -9857,7 +9857,7 @@
     </row>
     <row r="86" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>114</v>
+        <v>64</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -9952,7 +9952,7 @@
     </row>
     <row r="87" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -10047,7 +10047,7 @@
     </row>
     <row r="88" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -10142,7 +10142,7 @@
     </row>
     <row r="89" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>117</v>
+        <v>67</v>
       </c>
       <c r="B89">
         <v>0</v>
@@ -10237,7 +10237,7 @@
     </row>
     <row r="90" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="B90">
         <v>0</v>
@@ -10332,7 +10332,7 @@
     </row>
     <row r="91" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -10427,7 +10427,7 @@
     </row>
     <row r="92" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -10522,7 +10522,7 @@
     </row>
     <row r="93" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -10617,7 +10617,7 @@
     </row>
     <row r="94" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>122</v>
+        <v>72</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -10712,7 +10712,7 @@
     </row>
     <row r="95" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>123</v>
+        <v>73</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -10807,7 +10807,7 @@
     </row>
     <row r="96" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>124</v>
+        <v>74</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -10902,7 +10902,7 @@
     </row>
     <row r="97" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>125</v>
+        <v>75</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -10997,7 +10997,7 @@
     </row>
     <row r="98" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>126</v>
+        <v>76</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -11092,7 +11092,7 @@
     </row>
     <row r="99" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>127</v>
+        <v>77</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -11187,7 +11187,7 @@
     </row>
     <row r="100" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="B100">
         <v>0</v>
@@ -11282,7 +11282,7 @@
     </row>
     <row r="101" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>129</v>
+        <v>79</v>
       </c>
       <c r="B101">
         <v>0</v>
@@ -11377,7 +11377,7 @@
     </row>
     <row r="102" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>130</v>
+        <v>80</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -11472,7 +11472,7 @@
     </row>
     <row r="103" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>131</v>
+        <v>81</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -11567,7 +11567,7 @@
     </row>
     <row r="104" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>132</v>
+        <v>82</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -11662,7 +11662,7 @@
     </row>
     <row r="105" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -11757,7 +11757,7 @@
     </row>
     <row r="106" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>134</v>
+        <v>84</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -11852,7 +11852,7 @@
     </row>
     <row r="107" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>135</v>
+        <v>85</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -11947,7 +11947,7 @@
     </row>
     <row r="108" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>136</v>
+        <v>86</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -12042,7 +12042,7 @@
     </row>
     <row r="109" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>137</v>
+        <v>87</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -12137,7 +12137,7 @@
     </row>
     <row r="110" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>138</v>
+        <v>88</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -12232,7 +12232,7 @@
     </row>
     <row r="111" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="B111">
         <v>0</v>
@@ -12327,7 +12327,7 @@
     </row>
     <row r="112" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -12422,7 +12422,7 @@
     </row>
     <row r="113" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>141</v>
+        <v>91</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -12517,7 +12517,7 @@
     </row>
     <row r="114" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>142</v>
+        <v>92</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -12612,7 +12612,7 @@
     </row>
     <row r="115" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>143</v>
+        <v>93</v>
       </c>
       <c r="B115">
         <v>0</v>
@@ -12707,7 +12707,7 @@
     </row>
     <row r="116" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>144</v>
+        <v>94</v>
       </c>
       <c r="B116">
         <v>0</v>
@@ -12802,7 +12802,7 @@
     </row>
     <row r="117" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>145</v>
+        <v>95</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -12897,7 +12897,7 @@
     </row>
     <row r="118" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>146</v>
+        <v>96</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -12992,7 +12992,7 @@
     </row>
     <row r="119" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>147</v>
+        <v>97</v>
       </c>
       <c r="B119">
         <v>0</v>
@@ -13087,7 +13087,7 @@
     </row>
     <row r="120" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>148</v>
+        <v>98</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -13182,7 +13182,7 @@
     </row>
     <row r="121" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>149</v>
+        <v>99</v>
       </c>
       <c r="B121">
         <v>0</v>
@@ -13277,7 +13277,7 @@
     </row>
     <row r="122" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -13372,7 +13372,7 @@
     </row>
     <row r="123" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>151</v>
+        <v>101</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -13467,7 +13467,7 @@
     </row>
     <row r="124" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>152</v>
+        <v>102</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -13562,7 +13562,7 @@
     </row>
     <row r="125" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>153</v>
+        <v>103</v>
       </c>
       <c r="B125">
         <v>0</v>
@@ -13657,7 +13657,7 @@
     </row>
     <row r="126" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>154</v>
+        <v>104</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -13752,7 +13752,7 @@
     </row>
     <row r="127" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>155</v>
+        <v>105</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -13847,7 +13847,7 @@
     </row>
     <row r="128" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
-        <v>156</v>
+        <v>106</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -13942,7 +13942,7 @@
     </row>
     <row r="129" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
-        <v>157</v>
+        <v>107</v>
       </c>
       <c r="B129">
         <v>0</v>
@@ -14037,7 +14037,7 @@
     </row>
     <row r="130" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
-        <v>158</v>
+        <v>108</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -14132,7 +14132,7 @@
     </row>
     <row r="131" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>159</v>
+        <v>109</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -14227,7 +14227,7 @@
     </row>
     <row r="132" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
-        <v>160</v>
+        <v>110</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -14322,7 +14322,7 @@
     </row>
     <row r="133" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
-        <v>161</v>
+        <v>111</v>
       </c>
       <c r="B133">
         <v>0</v>
@@ -14417,7 +14417,7 @@
     </row>
     <row r="134" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>162</v>
+        <v>112</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -14512,7 +14512,7 @@
     </row>
     <row r="135" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -14607,7 +14607,7 @@
     </row>
     <row r="136" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -14702,7 +14702,7 @@
     </row>
     <row r="137" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B137">
         <v>0</v>
@@ -14797,7 +14797,7 @@
     </row>
     <row r="138" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>166</v>
+        <v>116</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -14892,7 +14892,7 @@
     </row>
     <row r="139" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="B139">
         <v>0</v>
@@ -14987,7 +14987,7 @@
     </row>
     <row r="140" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>168</v>
+        <v>118</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -15082,7 +15082,7 @@
     </row>
     <row r="141" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>169</v>
+        <v>119</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -15177,7 +15177,7 @@
     </row>
     <row r="142" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>170</v>
+        <v>120</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -15272,7 +15272,7 @@
     </row>
     <row r="143" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>171</v>
+        <v>121</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -15367,7 +15367,7 @@
     </row>
     <row r="144" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>172</v>
+        <v>122</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -15462,7 +15462,7 @@
     </row>
     <row r="145" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B145">
         <v>0</v>
@@ -15557,7 +15557,7 @@
     </row>
     <row r="146" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -15652,7 +15652,7 @@
     </row>
     <row r="147" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>175</v>
+        <v>125</v>
       </c>
       <c r="B147">
         <v>10</v>
@@ -15747,7 +15747,7 @@
     </row>
     <row r="148" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>176</v>
+        <v>126</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -15842,7 +15842,7 @@
     </row>
     <row r="149" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>177</v>
+        <v>127</v>
       </c>
       <c r="B149">
         <v>0</v>
@@ -15937,7 +15937,7 @@
     </row>
     <row r="150" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>178</v>
+        <v>128</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -16032,7 +16032,7 @@
     </row>
     <row r="151" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>179</v>
+        <v>129</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -16127,7 +16127,7 @@
     </row>
     <row r="152" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>180</v>
+        <v>130</v>
       </c>
       <c r="B152">
         <v>11</v>
@@ -16222,7 +16222,7 @@
     </row>
     <row r="153" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>181</v>
+        <v>131</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -16317,7 +16317,7 @@
     </row>
     <row r="154" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>182</v>
+        <v>132</v>
       </c>
       <c r="B154">
         <v>5</v>
@@ -16412,7 +16412,7 @@
     </row>
     <row r="155" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>183</v>
+        <v>133</v>
       </c>
       <c r="B155">
         <v>8</v>
@@ -16507,7 +16507,7 @@
     </row>
     <row r="156" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>184</v>
+        <v>134</v>
       </c>
       <c r="B156">
         <v>1</v>
@@ -16602,7 +16602,7 @@
     </row>
     <row r="157" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>185</v>
+        <v>135</v>
       </c>
       <c r="B157">
         <v>0</v>
@@ -16697,7 +16697,7 @@
     </row>
     <row r="158" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>186</v>
+        <v>136</v>
       </c>
       <c r="B158">
         <v>36</v>
@@ -16792,7 +16792,7 @@
     </row>
     <row r="159" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>187</v>
+        <v>137</v>
       </c>
       <c r="B159">
         <v>23</v>
@@ -16887,7 +16887,7 @@
     </row>
     <row r="160" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>188</v>
+        <v>138</v>
       </c>
       <c r="B160">
         <v>2</v>
@@ -16982,7 +16982,7 @@
     </row>
     <row r="161" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>189</v>
+        <v>139</v>
       </c>
       <c r="B161">
         <v>10</v>
@@ -17077,7 +17077,7 @@
     </row>
     <row r="162" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>190</v>
+        <v>140</v>
       </c>
       <c r="B162">
         <v>64</v>
@@ -17172,7 +17172,7 @@
     </row>
     <row r="163" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="B163">
         <v>14</v>
@@ -17267,7 +17267,7 @@
     </row>
     <row r="164" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>192</v>
+        <v>142</v>
       </c>
       <c r="B164">
         <v>63</v>
@@ -17362,7 +17362,7 @@
     </row>
     <row r="165" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>193</v>
+        <v>143</v>
       </c>
       <c r="B165">
         <v>84</v>
@@ -17457,7 +17457,7 @@
     </row>
     <row r="166" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>194</v>
+        <v>144</v>
       </c>
       <c r="B166">
         <v>2</v>
@@ -17552,7 +17552,7 @@
     </row>
     <row r="167" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>195</v>
+        <v>145</v>
       </c>
       <c r="B167">
         <v>22</v>
@@ -17647,7 +17647,7 @@
     </row>
     <row r="168" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>196</v>
+        <v>146</v>
       </c>
       <c r="B168">
         <v>25</v>
@@ -17742,7 +17742,7 @@
     </row>
     <row r="169" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>197</v>
+        <v>147</v>
       </c>
       <c r="B169">
         <v>28</v>
@@ -17837,7 +17837,7 @@
     </row>
     <row r="170" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>198</v>
+        <v>148</v>
       </c>
       <c r="B170">
         <v>3</v>
@@ -17932,7 +17932,7 @@
     </row>
     <row r="171" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="B171">
         <v>84</v>
@@ -18027,7 +18027,7 @@
     </row>
     <row r="172" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -18122,7 +18122,7 @@
     </row>
     <row r="173" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>201</v>
+        <v>151</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -18217,7 +18217,7 @@
     </row>
     <row r="174" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -18312,7 +18312,7 @@
     </row>
     <row r="175" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>203</v>
+        <v>153</v>
       </c>
       <c r="B175">
         <v>0</v>
@@ -18407,7 +18407,7 @@
     </row>
     <row r="176" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>204</v>
+        <v>154</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -18502,7 +18502,7 @@
     </row>
     <row r="177" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>205</v>
+        <v>155</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -18597,7 +18597,7 @@
     </row>
     <row r="178" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>206</v>
+        <v>156</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -18692,7 +18692,7 @@
     </row>
     <row r="179" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>207</v>
+        <v>157</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -18787,7 +18787,7 @@
     </row>
     <row r="180" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>208</v>
+        <v>158</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -18882,7 +18882,7 @@
     </row>
     <row r="181" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>209</v>
+        <v>159</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -18977,7 +18977,7 @@
     </row>
     <row r="182" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>210</v>
+        <v>160</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -19072,7 +19072,7 @@
     </row>
     <row r="183" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>211</v>
+        <v>161</v>
       </c>
       <c r="B183">
         <v>0</v>
@@ -19167,7 +19167,7 @@
     </row>
     <row r="184" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>212</v>
+        <v>162</v>
       </c>
       <c r="B184">
         <v>1</v>
@@ -19262,7 +19262,7 @@
     </row>
     <row r="185" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>213</v>
+        <v>163</v>
       </c>
       <c r="B185">
         <v>2</v>
@@ -19357,7 +19357,7 @@
     </row>
     <row r="186" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>214</v>
+        <v>164</v>
       </c>
       <c r="B186">
         <v>3</v>
@@ -19452,7 +19452,7 @@
     </row>
     <row r="187" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>215</v>
+        <v>165</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -19547,7 +19547,7 @@
     </row>
     <row r="188" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>216</v>
+        <v>166</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -19642,7 +19642,7 @@
     </row>
     <row r="189" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>217</v>
+        <v>167</v>
       </c>
       <c r="B189">
         <v>0</v>
@@ -19737,7 +19737,7 @@
     </row>
     <row r="190" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>218</v>
+        <v>168</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -19832,7 +19832,7 @@
     </row>
     <row r="191" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>219</v>
+        <v>169</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -19927,7 +19927,7 @@
     </row>
     <row r="192" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -20022,7 +20022,7 @@
     </row>
     <row r="193" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>221</v>
+        <v>171</v>
       </c>
       <c r="B193">
         <v>3</v>
@@ -20117,7 +20117,7 @@
     </row>
     <row r="194" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>222</v>
+        <v>172</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -20212,7 +20212,7 @@
     </row>
     <row r="195" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>223</v>
+        <v>173</v>
       </c>
       <c r="B195">
         <v>12</v>
@@ -20307,7 +20307,7 @@
     </row>
     <row r="196" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>224</v>
+        <v>174</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -20402,7 +20402,7 @@
     </row>
     <row r="197" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
-        <v>225</v>
+        <v>175</v>
       </c>
       <c r="B197">
         <v>0</v>
@@ -20497,7 +20497,7 @@
     </row>
     <row r="198" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>226</v>
+        <v>176</v>
       </c>
       <c r="B198">
         <v>5</v>
@@ -20592,7 +20592,7 @@
     </row>
     <row r="199" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>227</v>
+        <v>177</v>
       </c>
       <c r="B199">
         <v>0</v>
@@ -20687,7 +20687,7 @@
     </row>
     <row r="200" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>228</v>
+        <v>178</v>
       </c>
       <c r="B200">
         <v>27</v>
@@ -20782,7 +20782,7 @@
     </row>
     <row r="201" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>229</v>
+        <v>179</v>
       </c>
       <c r="B201">
         <v>7</v>
@@ -20877,7 +20877,7 @@
     </row>
     <row r="202" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>230</v>
+        <v>180</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -20972,7 +20972,7 @@
     </row>
     <row r="203" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>231</v>
+        <v>181</v>
       </c>
       <c r="B203">
         <v>0</v>
@@ -21067,7 +21067,7 @@
     </row>
     <row r="204" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>232</v>
+        <v>182</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -21162,7 +21162,7 @@
     </row>
     <row r="205" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>233</v>
+        <v>183</v>
       </c>
       <c r="B205">
         <v>0</v>
@@ -21257,7 +21257,7 @@
     </row>
     <row r="206" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>234</v>
+        <v>184</v>
       </c>
       <c r="B206">
         <v>0</v>
@@ -21352,7 +21352,7 @@
     </row>
     <row r="207" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>235</v>
+        <v>185</v>
       </c>
       <c r="B207">
         <v>0</v>
@@ -21447,7 +21447,7 @@
     </row>
     <row r="208" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
-        <v>236</v>
+        <v>186</v>
       </c>
       <c r="B208">
         <v>0</v>
@@ -21542,7 +21542,7 @@
     </row>
     <row r="209" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
-        <v>237</v>
+        <v>187</v>
       </c>
       <c r="B209">
         <v>0</v>
@@ -21637,7 +21637,7 @@
     </row>
     <row r="210" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
-        <v>238</v>
+        <v>188</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -21732,7 +21732,7 @@
     </row>
     <row r="211" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
-        <v>239</v>
+        <v>189</v>
       </c>
       <c r="B211">
         <v>0</v>
@@ -21827,7 +21827,7 @@
     </row>
     <row r="212" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
-        <v>240</v>
+        <v>190</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -21922,7 +21922,7 @@
     </row>
     <row r="213" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
-        <v>241</v>
+        <v>191</v>
       </c>
       <c r="B213">
         <v>0</v>
@@ -22017,7 +22017,7 @@
     </row>
     <row r="214" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
-        <v>242</v>
+        <v>192</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -22112,7 +22112,7 @@
     </row>
     <row r="215" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="B215">
         <v>0</v>
@@ -22207,7 +22207,7 @@
     </row>
     <row r="216" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
-        <v>244</v>
+        <v>194</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -22302,7 +22302,7 @@
     </row>
     <row r="217" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B217">
         <v>0</v>
@@ -22397,7 +22397,7 @@
     </row>
     <row r="218" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -22492,7 +22492,7 @@
     </row>
     <row r="219" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
-        <v>247</v>
+        <v>197</v>
       </c>
       <c r="B219">
         <v>0</v>
@@ -22587,7 +22587,7 @@
     </row>
     <row r="220" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
-        <v>248</v>
+        <v>198</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -22682,7 +22682,7 @@
     </row>
     <row r="221" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
-        <v>249</v>
+        <v>199</v>
       </c>
       <c r="B221">
         <v>0</v>
@@ -22777,7 +22777,7 @@
     </row>
     <row r="222" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -22872,7 +22872,7 @@
     </row>
     <row r="223" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
-        <v>251</v>
+        <v>201</v>
       </c>
       <c r="B223">
         <v>0</v>
@@ -22967,7 +22967,7 @@
     </row>
     <row r="224" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
-        <v>252</v>
+        <v>202</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -23062,7 +23062,7 @@
     </row>
     <row r="225" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
-        <v>253</v>
+        <v>203</v>
       </c>
       <c r="B225">
         <v>0</v>
@@ -23157,7 +23157,7 @@
     </row>
     <row r="226" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
-        <v>254</v>
+        <v>204</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -23252,7 +23252,7 @@
     </row>
     <row r="227" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
-        <v>255</v>
+        <v>205</v>
       </c>
       <c r="B227">
         <v>0</v>
@@ -23347,7 +23347,7 @@
     </row>
     <row r="228" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
-        <v>256</v>
+        <v>206</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -23442,7 +23442,7 @@
     </row>
     <row r="229" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
-        <v>257</v>
+        <v>207</v>
       </c>
       <c r="B229">
         <v>0</v>
@@ -23537,7 +23537,7 @@
     </row>
     <row r="230" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
-        <v>258</v>
+        <v>208</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -23632,7 +23632,7 @@
     </row>
     <row r="231" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
-        <v>259</v>
+        <v>209</v>
       </c>
       <c r="B231">
         <v>0</v>
@@ -23727,7 +23727,7 @@
     </row>
     <row r="232" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
-        <v>260</v>
+        <v>210</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -23822,7 +23822,7 @@
     </row>
     <row r="233" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
-        <v>261</v>
+        <v>211</v>
       </c>
       <c r="B233">
         <v>0</v>
@@ -23917,7 +23917,7 @@
     </row>
     <row r="234" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
-        <v>262</v>
+        <v>212</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -24012,7 +24012,7 @@
     </row>
     <row r="235" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
-        <v>263</v>
+        <v>213</v>
       </c>
       <c r="B235">
         <v>0</v>
@@ -24107,7 +24107,7 @@
     </row>
     <row r="236" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
-        <v>264</v>
+        <v>214</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -24202,7 +24202,7 @@
     </row>
     <row r="237" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
-        <v>265</v>
+        <v>215</v>
       </c>
       <c r="B237">
         <v>0</v>
@@ -24297,7 +24297,7 @@
     </row>
     <row r="238" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
-        <v>266</v>
+        <v>216</v>
       </c>
       <c r="B238">
         <v>0</v>
@@ -24392,7 +24392,7 @@
     </row>
     <row r="239" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
-        <v>267</v>
+        <v>217</v>
       </c>
       <c r="B239">
         <v>0</v>
@@ -24487,7 +24487,7 @@
     </row>
     <row r="240" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
-        <v>268</v>
+        <v>218</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -24582,7 +24582,7 @@
     </row>
     <row r="241" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
-        <v>269</v>
+        <v>219</v>
       </c>
       <c r="B241">
         <v>0</v>
@@ -24677,7 +24677,7 @@
     </row>
     <row r="242" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
-        <v>270</v>
+        <v>220</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -24772,7 +24772,7 @@
     </row>
     <row r="243" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
-        <v>271</v>
+        <v>221</v>
       </c>
       <c r="B243">
         <v>0</v>
@@ -24867,7 +24867,7 @@
     </row>
     <row r="244" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
-        <v>272</v>
+        <v>222</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -24962,7 +24962,7 @@
     </row>
     <row r="245" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
-        <v>273</v>
+        <v>223</v>
       </c>
       <c r="B245">
         <v>0</v>
@@ -25057,7 +25057,7 @@
     </row>
     <row r="246" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
-        <v>274</v>
+        <v>224</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -25152,7 +25152,7 @@
     </row>
     <row r="247" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
-        <v>275</v>
+        <v>225</v>
       </c>
       <c r="B247">
         <v>0</v>
@@ -25247,7 +25247,7 @@
     </row>
     <row r="248" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
-        <v>276</v>
+        <v>226</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -25342,7 +25342,7 @@
     </row>
     <row r="249" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
-        <v>277</v>
+        <v>227</v>
       </c>
       <c r="B249">
         <v>0</v>
@@ -25437,7 +25437,7 @@
     </row>
     <row r="250" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
-        <v>278</v>
+        <v>228</v>
       </c>
       <c r="B250">
         <v>0</v>
@@ -25532,7 +25532,7 @@
     </row>
     <row r="251" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
-        <v>279</v>
+        <v>229</v>
       </c>
       <c r="B251">
         <v>0</v>
@@ -25627,7 +25627,7 @@
     </row>
     <row r="252" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
-        <v>280</v>
+        <v>230</v>
       </c>
       <c r="B252">
         <v>0</v>
@@ -25722,7 +25722,7 @@
     </row>
     <row r="253" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
-        <v>281</v>
+        <v>231</v>
       </c>
       <c r="B253">
         <v>0</v>
@@ -25817,7 +25817,7 @@
     </row>
     <row r="254" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
-        <v>282</v>
+        <v>232</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -25912,7 +25912,7 @@
     </row>
     <row r="255" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
-        <v>283</v>
+        <v>233</v>
       </c>
       <c r="B255">
         <v>0</v>
@@ -26007,7 +26007,7 @@
     </row>
     <row r="256" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
-        <v>284</v>
+        <v>234</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -26102,7 +26102,7 @@
     </row>
     <row r="257" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
-        <v>285</v>
+        <v>235</v>
       </c>
       <c r="B257">
         <v>0</v>
@@ -26197,7 +26197,7 @@
     </row>
     <row r="258" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B258">
         <v>0</v>
@@ -26292,7 +26292,7 @@
     </row>
     <row r="259" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
-        <v>287</v>
+        <v>237</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -26387,7 +26387,7 @@
     </row>
     <row r="260" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
-        <v>288</v>
+        <v>238</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -26482,7 +26482,7 @@
     </row>
     <row r="261" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
-        <v>289</v>
+        <v>239</v>
       </c>
       <c r="B261">
         <v>0</v>
@@ -26577,7 +26577,7 @@
     </row>
     <row r="262" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
-        <v>290</v>
+        <v>240</v>
       </c>
       <c r="B262">
         <v>0</v>
@@ -26672,7 +26672,7 @@
     </row>
     <row r="263" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
-        <v>291</v>
+        <v>241</v>
       </c>
       <c r="B263">
         <v>0</v>
@@ -26767,7 +26767,7 @@
     </row>
     <row r="264" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
-        <v>292</v>
+        <v>242</v>
       </c>
       <c r="B264">
         <v>0</v>
@@ -26862,7 +26862,7 @@
     </row>
     <row r="265" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
-        <v>293</v>
+        <v>243</v>
       </c>
       <c r="B265">
         <v>0</v>
@@ -26957,7 +26957,7 @@
     </row>
     <row r="266" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
-        <v>294</v>
+        <v>244</v>
       </c>
       <c r="B266">
         <v>0</v>
@@ -27052,7 +27052,7 @@
     </row>
     <row r="267" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
-        <v>295</v>
+        <v>245</v>
       </c>
       <c r="B267">
         <v>0</v>
@@ -27147,7 +27147,7 @@
     </row>
     <row r="268" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
-        <v>296</v>
+        <v>246</v>
       </c>
       <c r="B268">
         <v>0</v>
@@ -27242,7 +27242,7 @@
     </row>
     <row r="269" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
-        <v>297</v>
+        <v>247</v>
       </c>
       <c r="B269">
         <v>0</v>
@@ -27337,7 +27337,7 @@
     </row>
     <row r="270" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
-        <v>298</v>
+        <v>248</v>
       </c>
       <c r="B270">
         <v>0</v>
@@ -27432,7 +27432,7 @@
     </row>
     <row r="271" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
-        <v>299</v>
+        <v>249</v>
       </c>
       <c r="B271">
         <v>0</v>
@@ -27527,7 +27527,7 @@
     </row>
     <row r="272" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="B272">
         <v>0</v>
@@ -27622,7 +27622,7 @@
     </row>
     <row r="273" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
-        <v>301</v>
+        <v>251</v>
       </c>
       <c r="B273">
         <v>0</v>
@@ -27717,7 +27717,7 @@
     </row>
     <row r="274" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
-        <v>302</v>
+        <v>252</v>
       </c>
       <c r="B274">
         <v>0</v>
@@ -27812,7 +27812,7 @@
     </row>
     <row r="275" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
-        <v>303</v>
+        <v>253</v>
       </c>
       <c r="B275">
         <v>0</v>
@@ -27907,7 +27907,7 @@
     </row>
     <row r="276" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
-        <v>304</v>
+        <v>254</v>
       </c>
       <c r="B276">
         <v>0</v>
@@ -28002,7 +28002,7 @@
     </row>
     <row r="277" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
-        <v>305</v>
+        <v>255</v>
       </c>
       <c r="B277">
         <v>0</v>
@@ -28097,7 +28097,7 @@
     </row>
     <row r="278" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
-        <v>306</v>
+        <v>256</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -28192,7 +28192,7 @@
     </row>
     <row r="279" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
-        <v>307</v>
+        <v>257</v>
       </c>
       <c r="B279">
         <v>0</v>
@@ -28287,7 +28287,7 @@
     </row>
     <row r="280" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
-        <v>308</v>
+        <v>258</v>
       </c>
       <c r="B280">
         <v>0</v>
@@ -28382,7 +28382,7 @@
     </row>
     <row r="281" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
-        <v>309</v>
+        <v>259</v>
       </c>
       <c r="B281">
         <v>0</v>
@@ -28477,7 +28477,7 @@
     </row>
     <row r="282" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -28572,7 +28572,7 @@
     </row>
     <row r="283" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
-        <v>311</v>
+        <v>261</v>
       </c>
       <c r="B283">
         <v>0</v>
@@ -28667,7 +28667,7 @@
     </row>
     <row r="284" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
-        <v>312</v>
+        <v>262</v>
       </c>
       <c r="B284">
         <v>0</v>
@@ -28762,7 +28762,7 @@
     </row>
     <row r="285" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
-        <v>313</v>
+        <v>263</v>
       </c>
       <c r="B285">
         <v>0</v>
@@ -28857,7 +28857,7 @@
     </row>
     <row r="286" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
-        <v>314</v>
+        <v>264</v>
       </c>
       <c r="B286">
         <v>0</v>
@@ -28952,7 +28952,7 @@
     </row>
     <row r="287" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
-        <v>315</v>
+        <v>265</v>
       </c>
       <c r="B287">
         <v>0</v>
@@ -29047,7 +29047,7 @@
     </row>
     <row r="288" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
-        <v>316</v>
+        <v>266</v>
       </c>
       <c r="B288">
         <v>0</v>
@@ -29142,7 +29142,7 @@
     </row>
     <row r="289" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
-        <v>317</v>
+        <v>267</v>
       </c>
       <c r="B289">
         <v>0</v>
@@ -29237,7 +29237,7 @@
     </row>
     <row r="290" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
-        <v>318</v>
+        <v>268</v>
       </c>
       <c r="B290">
         <v>0</v>
@@ -29332,7 +29332,7 @@
     </row>
     <row r="291" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
-        <v>319</v>
+        <v>269</v>
       </c>
       <c r="B291">
         <v>0</v>
@@ -29427,7 +29427,7 @@
     </row>
     <row r="292" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
-        <v>320</v>
+        <v>270</v>
       </c>
       <c r="B292">
         <v>0</v>
@@ -29522,7 +29522,7 @@
     </row>
     <row r="293" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
-        <v>321</v>
+        <v>271</v>
       </c>
       <c r="B293">
         <v>6</v>
@@ -29617,7 +29617,7 @@
     </row>
     <row r="294" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
-        <v>322</v>
+        <v>272</v>
       </c>
       <c r="B294">
         <v>0</v>
@@ -29712,7 +29712,7 @@
     </row>
     <row r="295" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
-        <v>323</v>
+        <v>273</v>
       </c>
       <c r="B295">
         <v>0</v>
@@ -29807,7 +29807,7 @@
     </row>
     <row r="296" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
-        <v>324</v>
+        <v>274</v>
       </c>
       <c r="B296">
         <v>0</v>
@@ -29902,7 +29902,7 @@
     </row>
     <row r="297" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
-        <v>325</v>
+        <v>275</v>
       </c>
       <c r="B297">
         <v>0</v>
@@ -29997,7 +29997,7 @@
     </row>
     <row r="298" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
-        <v>326</v>
+        <v>276</v>
       </c>
       <c r="B298">
         <v>0</v>
@@ -30092,7 +30092,7 @@
     </row>
     <row r="299" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
-        <v>327</v>
+        <v>277</v>
       </c>
       <c r="B299">
         <v>0</v>
@@ -30187,7 +30187,7 @@
     </row>
     <row r="300" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
-        <v>328</v>
+        <v>278</v>
       </c>
       <c r="B300">
         <v>0</v>
@@ -30282,7 +30282,7 @@
     </row>
     <row r="301" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
-        <v>329</v>
+        <v>279</v>
       </c>
       <c r="B301">
         <v>0</v>
@@ -30377,7 +30377,7 @@
     </row>
     <row r="302" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
-        <v>330</v>
+        <v>280</v>
       </c>
       <c r="B302">
         <v>0</v>
@@ -30472,7 +30472,7 @@
     </row>
     <row r="303" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
-        <v>331</v>
+        <v>281</v>
       </c>
       <c r="B303">
         <v>1</v>
@@ -30567,7 +30567,7 @@
     </row>
     <row r="304" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
-        <v>332</v>
+        <v>282</v>
       </c>
       <c r="B304">
         <v>0</v>
@@ -30662,7 +30662,7 @@
     </row>
     <row r="305" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
-        <v>333</v>
+        <v>283</v>
       </c>
       <c r="B305">
         <v>0</v>
@@ -30757,7 +30757,7 @@
     </row>
     <row r="306" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
-        <v>334</v>
+        <v>284</v>
       </c>
       <c r="B306">
         <v>0</v>
@@ -30852,7 +30852,7 @@
     </row>
     <row r="307" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
-        <v>335</v>
+        <v>285</v>
       </c>
       <c r="B307">
         <v>0</v>
@@ -30947,7 +30947,7 @@
     </row>
     <row r="308" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
-        <v>336</v>
+        <v>286</v>
       </c>
       <c r="B308">
         <v>0</v>
@@ -31042,7 +31042,7 @@
     </row>
     <row r="309" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
-        <v>337</v>
+        <v>287</v>
       </c>
       <c r="B309">
         <v>0</v>
@@ -31137,7 +31137,7 @@
     </row>
     <row r="310" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
-        <v>338</v>
+        <v>288</v>
       </c>
       <c r="B310">
         <v>0</v>
@@ -31232,7 +31232,7 @@
     </row>
     <row r="311" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
-        <v>339</v>
+        <v>289</v>
       </c>
       <c r="B311">
         <v>0</v>
@@ -31327,7 +31327,7 @@
     </row>
     <row r="312" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
-        <v>340</v>
+        <v>290</v>
       </c>
       <c r="B312">
         <v>0</v>
@@ -31422,7 +31422,7 @@
     </row>
     <row r="313" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
-        <v>341</v>
+        <v>291</v>
       </c>
       <c r="B313">
         <v>0</v>
@@ -31517,7 +31517,7 @@
     </row>
     <row r="314" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
-        <v>342</v>
+        <v>292</v>
       </c>
       <c r="B314">
         <v>0</v>
@@ -31612,7 +31612,7 @@
     </row>
     <row r="315" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
-        <v>343</v>
+        <v>293</v>
       </c>
       <c r="B315">
         <v>0</v>
@@ -31707,7 +31707,7 @@
     </row>
     <row r="316" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
-        <v>344</v>
+        <v>294</v>
       </c>
       <c r="B316">
         <v>0</v>
@@ -31802,7 +31802,7 @@
     </row>
     <row r="317" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
-        <v>345</v>
+        <v>295</v>
       </c>
       <c r="B317">
         <v>0</v>
@@ -31897,7 +31897,7 @@
     </row>
     <row r="318" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
-        <v>346</v>
+        <v>296</v>
       </c>
       <c r="B318">
         <v>0</v>
@@ -31992,7 +31992,7 @@
     </row>
     <row r="319" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
-        <v>347</v>
+        <v>297</v>
       </c>
       <c r="B319">
         <v>0</v>
@@ -32087,7 +32087,7 @@
     </row>
     <row r="320" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
-        <v>348</v>
+        <v>298</v>
       </c>
       <c r="B320">
         <v>0</v>
@@ -32182,7 +32182,7 @@
     </row>
     <row r="321" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
-        <v>349</v>
+        <v>299</v>
       </c>
       <c r="B321">
         <v>0</v>
@@ -32277,7 +32277,7 @@
     </row>
     <row r="322" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="B322">
         <v>0</v>
@@ -32372,7 +32372,7 @@
     </row>
     <row r="323" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
-        <v>351</v>
+        <v>301</v>
       </c>
       <c r="B323">
         <v>0</v>
@@ -32467,7 +32467,7 @@
     </row>
     <row r="324" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
-        <v>352</v>
+        <v>302</v>
       </c>
       <c r="B324">
         <v>0</v>
@@ -32562,7 +32562,7 @@
     </row>
     <row r="325" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
-        <v>353</v>
+        <v>303</v>
       </c>
       <c r="B325">
         <v>0</v>
@@ -32657,7 +32657,7 @@
     </row>
     <row r="326" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
-        <v>354</v>
+        <v>304</v>
       </c>
       <c r="B326">
         <v>0</v>
@@ -32752,7 +32752,7 @@
     </row>
     <row r="327" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
-        <v>355</v>
+        <v>305</v>
       </c>
       <c r="B327">
         <v>0</v>
@@ -32847,7 +32847,7 @@
     </row>
     <row r="328" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
-        <v>356</v>
+        <v>306</v>
       </c>
       <c r="B328">
         <v>0</v>
@@ -32942,7 +32942,7 @@
     </row>
     <row r="329" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
-        <v>357</v>
+        <v>307</v>
       </c>
       <c r="B329">
         <v>0</v>
@@ -33037,7 +33037,7 @@
     </row>
     <row r="330" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
-        <v>358</v>
+        <v>308</v>
       </c>
       <c r="B330">
         <v>0</v>
@@ -33132,7 +33132,7 @@
     </row>
     <row r="331" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
-        <v>359</v>
+        <v>309</v>
       </c>
       <c r="B331">
         <v>0</v>
@@ -33227,7 +33227,7 @@
     </row>
     <row r="332" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
-        <v>360</v>
+        <v>310</v>
       </c>
       <c r="B332">
         <v>0</v>
@@ -33322,7 +33322,7 @@
     </row>
     <row r="333" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
-        <v>361</v>
+        <v>311</v>
       </c>
       <c r="B333">
         <v>0</v>
@@ -33417,7 +33417,7 @@
     </row>
     <row r="334" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
-        <v>362</v>
+        <v>312</v>
       </c>
       <c r="B334">
         <v>5</v>
@@ -33512,7 +33512,7 @@
     </row>
     <row r="335" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
-        <v>363</v>
+        <v>313</v>
       </c>
       <c r="B335">
         <v>0</v>
@@ -33607,7 +33607,7 @@
     </row>
     <row r="336" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
-        <v>364</v>
+        <v>314</v>
       </c>
       <c r="B336">
         <v>1</v>
@@ -33702,7 +33702,7 @@
     </row>
     <row r="337" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
-        <v>365</v>
+        <v>315</v>
       </c>
       <c r="B337">
         <v>0</v>
@@ -33797,7 +33797,7 @@
     </row>
     <row r="338" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
-        <v>366</v>
+        <v>316</v>
       </c>
       <c r="B338">
         <v>0</v>
@@ -33892,7 +33892,7 @@
     </row>
     <row r="339" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
-        <v>367</v>
+        <v>317</v>
       </c>
       <c r="B339">
         <v>0</v>
@@ -33987,7 +33987,7 @@
     </row>
     <row r="340" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
-        <v>368</v>
+        <v>318</v>
       </c>
       <c r="B340">
         <v>0</v>
@@ -34082,7 +34082,7 @@
     </row>
     <row r="341" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
-        <v>369</v>
+        <v>319</v>
       </c>
       <c r="B341">
         <v>0</v>
@@ -34177,7 +34177,7 @@
     </row>
     <row r="342" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
-        <v>370</v>
+        <v>320</v>
       </c>
       <c r="B342">
         <v>0</v>
@@ -34272,7 +34272,7 @@
     </row>
     <row r="343" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
-        <v>371</v>
+        <v>321</v>
       </c>
       <c r="B343">
         <v>0</v>
@@ -34367,7 +34367,7 @@
     </row>
     <row r="344" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
-        <v>372</v>
+        <v>322</v>
       </c>
       <c r="B344">
         <v>0</v>
@@ -34462,7 +34462,7 @@
     </row>
     <row r="345" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
-        <v>373</v>
+        <v>323</v>
       </c>
       <c r="B345">
         <v>0</v>
@@ -34557,7 +34557,7 @@
     </row>
     <row r="346" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
-        <v>374</v>
+        <v>324</v>
       </c>
       <c r="B346">
         <v>0</v>
@@ -34652,7 +34652,7 @@
     </row>
     <row r="347" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
-        <v>375</v>
+        <v>325</v>
       </c>
       <c r="B347">
         <v>0</v>
@@ -34747,7 +34747,7 @@
     </row>
     <row r="348" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
-        <v>376</v>
+        <v>326</v>
       </c>
       <c r="B348">
         <v>0</v>
@@ -34842,7 +34842,7 @@
     </row>
     <row r="349" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
-        <v>377</v>
+        <v>327</v>
       </c>
       <c r="B349">
         <v>0</v>
@@ -34937,7 +34937,7 @@
     </row>
     <row r="350" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="B350">
         <v>0</v>
@@ -35032,7 +35032,7 @@
     </row>
     <row r="351" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
-        <v>379</v>
+        <v>329</v>
       </c>
       <c r="B351">
         <v>0</v>
@@ -35127,7 +35127,7 @@
     </row>
     <row r="352" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
-        <v>380</v>
+        <v>330</v>
       </c>
       <c r="B352">
         <v>0</v>
@@ -35222,7 +35222,7 @@
     </row>
     <row r="353" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
-        <v>381</v>
+        <v>331</v>
       </c>
       <c r="B353">
         <v>0</v>
@@ -35317,7 +35317,7 @@
     </row>
     <row r="354" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
-        <v>382</v>
+        <v>332</v>
       </c>
       <c r="B354">
         <v>0</v>
@@ -35412,7 +35412,7 @@
     </row>
     <row r="355" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
-        <v>383</v>
+        <v>333</v>
       </c>
       <c r="B355">
         <v>0</v>
@@ -35507,7 +35507,7 @@
     </row>
     <row r="356" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
-        <v>384</v>
+        <v>334</v>
       </c>
       <c r="B356">
         <v>0</v>
@@ -35602,7 +35602,7 @@
     </row>
     <row r="357" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
-        <v>385</v>
+        <v>335</v>
       </c>
       <c r="B357">
         <v>0</v>
@@ -35697,7 +35697,7 @@
     </row>
     <row r="358" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
-        <v>386</v>
+        <v>336</v>
       </c>
       <c r="B358">
         <v>32</v>
@@ -35792,7 +35792,7 @@
     </row>
     <row r="359" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
-        <v>387</v>
+        <v>337</v>
       </c>
       <c r="B359">
         <v>14</v>
@@ -35887,7 +35887,7 @@
     </row>
     <row r="360" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
-        <v>388</v>
+        <v>338</v>
       </c>
       <c r="B360">
         <v>0</v>
@@ -35982,7 +35982,7 @@
     </row>
     <row r="361" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
-        <v>389</v>
+        <v>339</v>
       </c>
       <c r="B361">
         <v>0</v>
@@ -36077,7 +36077,7 @@
     </row>
     <row r="362" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
-        <v>390</v>
+        <v>340</v>
       </c>
       <c r="B362">
         <v>0</v>
@@ -36172,7 +36172,7 @@
     </row>
     <row r="363" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
-        <v>391</v>
+        <v>341</v>
       </c>
       <c r="B363">
         <v>0</v>
@@ -36267,7 +36267,7 @@
     </row>
     <row r="364" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
-        <v>392</v>
+        <v>342</v>
       </c>
       <c r="B364">
         <v>0</v>
@@ -36362,7 +36362,7 @@
     </row>
     <row r="365" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
-        <v>393</v>
+        <v>343</v>
       </c>
       <c r="B365">
         <v>0</v>
@@ -36457,7 +36457,7 @@
     </row>
     <row r="366" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
-        <v>394</v>
+        <v>344</v>
       </c>
       <c r="B366">
         <v>0</v>
@@ -36552,7 +36552,7 @@
     </row>
     <row r="367" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
-        <v>395</v>
+        <v>345</v>
       </c>
       <c r="B367">
         <v>0</v>
@@ -36647,7 +36647,7 @@
     </row>
     <row r="368" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
-        <v>396</v>
+        <v>346</v>
       </c>
       <c r="B368">
         <v>0</v>
@@ -36742,7 +36742,7 @@
     </row>
     <row r="369" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
-        <v>397</v>
+        <v>347</v>
       </c>
       <c r="B369">
         <v>0</v>
@@ -36837,7 +36837,7 @@
     </row>
     <row r="370" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
-        <v>398</v>
+        <v>348</v>
       </c>
       <c r="B370">
         <v>0</v>
@@ -36932,7 +36932,7 @@
     </row>
     <row r="371" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
-        <v>399</v>
+        <v>349</v>
       </c>
       <c r="B371">
         <v>0</v>
@@ -37027,7 +37027,7 @@
     </row>
     <row r="372" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
-        <v>400</v>
+        <v>350</v>
       </c>
       <c r="B372">
         <v>0</v>
@@ -37122,7 +37122,7 @@
     </row>
     <row r="373" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
-        <v>401</v>
+        <v>351</v>
       </c>
       <c r="B373">
         <v>5</v>
@@ -37217,7 +37217,7 @@
     </row>
     <row r="374" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
-        <v>402</v>
+        <v>352</v>
       </c>
       <c r="B374">
         <v>7</v>
@@ -37312,7 +37312,7 @@
     </row>
     <row r="375" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
-        <v>403</v>
+        <v>353</v>
       </c>
       <c r="B375">
         <v>0</v>
@@ -37407,7 +37407,7 @@
     </row>
     <row r="376" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
-        <v>404</v>
+        <v>354</v>
       </c>
       <c r="B376">
         <v>0</v>
@@ -37502,7 +37502,7 @@
     </row>
     <row r="377" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
-        <v>405</v>
+        <v>355</v>
       </c>
       <c r="B377">
         <v>0</v>
@@ -37597,7 +37597,7 @@
     </row>
     <row r="378" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
-        <v>406</v>
+        <v>356</v>
       </c>
       <c r="B378">
         <v>0</v>
@@ -37692,7 +37692,7 @@
     </row>
     <row r="379" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
-        <v>407</v>
+        <v>357</v>
       </c>
       <c r="B379">
         <v>0</v>
@@ -37787,7 +37787,7 @@
     </row>
     <row r="380" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
-        <v>408</v>
+        <v>358</v>
       </c>
       <c r="B380">
         <v>0</v>
@@ -37882,7 +37882,7 @@
     </row>
     <row r="381" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
-        <v>409</v>
+        <v>359</v>
       </c>
       <c r="B381">
         <v>0</v>
@@ -37977,7 +37977,7 @@
     </row>
     <row r="382" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
-        <v>410</v>
+        <v>360</v>
       </c>
       <c r="B382">
         <v>0</v>
@@ -38072,7 +38072,7 @@
     </row>
     <row r="383" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
-        <v>411</v>
+        <v>361</v>
       </c>
       <c r="B383">
         <v>8</v>
@@ -38167,7 +38167,7 @@
     </row>
     <row r="384" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
-        <v>412</v>
+        <v>362</v>
       </c>
       <c r="B384">
         <v>0</v>
@@ -38262,7 +38262,7 @@
     </row>
     <row r="385" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
-        <v>413</v>
+        <v>363</v>
       </c>
       <c r="B385">
         <v>1</v>
@@ -38357,7 +38357,7 @@
     </row>
     <row r="386" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
-        <v>414</v>
+        <v>364</v>
       </c>
       <c r="B386">
         <v>0</v>
@@ -38452,7 +38452,7 @@
     </row>
     <row r="387" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
-        <v>415</v>
+        <v>365</v>
       </c>
       <c r="B387">
         <v>12</v>
@@ -38547,7 +38547,7 @@
     </row>
     <row r="388" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
-        <v>416</v>
+        <v>366</v>
       </c>
       <c r="B388">
         <v>0</v>
@@ -38642,7 +38642,7 @@
     </row>
     <row r="389" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
-        <v>417</v>
+        <v>367</v>
       </c>
       <c r="B389">
         <v>10</v>
@@ -38737,7 +38737,7 @@
     </row>
     <row r="390" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
-        <v>418</v>
+        <v>368</v>
       </c>
       <c r="B390">
         <v>0</v>
@@ -38832,7 +38832,7 @@
     </row>
     <row r="391" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
-        <v>419</v>
+        <v>369</v>
       </c>
       <c r="B391">
         <v>0</v>
@@ -38927,7 +38927,7 @@
     </row>
     <row r="392" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
-        <v>420</v>
+        <v>370</v>
       </c>
       <c r="B392">
         <v>0</v>
@@ -39022,7 +39022,7 @@
     </row>
     <row r="393" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
-        <v>421</v>
+        <v>371</v>
       </c>
       <c r="B393">
         <v>0</v>
@@ -39117,7 +39117,7 @@
     </row>
     <row r="394" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
-        <v>422</v>
+        <v>372</v>
       </c>
       <c r="B394">
         <v>0</v>
@@ -39212,7 +39212,7 @@
     </row>
     <row r="395" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
-        <v>423</v>
+        <v>373</v>
       </c>
       <c r="B395">
         <v>0</v>
@@ -39307,7 +39307,7 @@
     </row>
     <row r="396" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
-        <v>424</v>
+        <v>374</v>
       </c>
       <c r="B396">
         <v>0</v>
@@ -39402,7 +39402,7 @@
     </row>
     <row r="397" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
-        <v>425</v>
+        <v>375</v>
       </c>
       <c r="B397">
         <v>0</v>
@@ -39497,7 +39497,7 @@
     </row>
     <row r="398" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
-        <v>426</v>
+        <v>376</v>
       </c>
       <c r="B398">
         <v>0</v>
@@ -39592,7 +39592,7 @@
     </row>
     <row r="399" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
-        <v>427</v>
+        <v>377</v>
       </c>
       <c r="B399">
         <v>0</v>
@@ -39687,7 +39687,7 @@
     </row>
     <row r="400" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
-        <v>428</v>
+        <v>378</v>
       </c>
       <c r="B400">
         <v>0</v>
@@ -39782,7 +39782,7 @@
     </row>
     <row r="401" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
-        <v>429</v>
+        <v>379</v>
       </c>
       <c r="B401">
         <v>0</v>
@@ -39877,7 +39877,7 @@
     </row>
     <row r="402" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
-        <v>430</v>
+        <v>380</v>
       </c>
       <c r="B402">
         <v>0</v>
@@ -39972,7 +39972,7 @@
     </row>
     <row r="403" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
-        <v>431</v>
+        <v>381</v>
       </c>
       <c r="B403">
         <v>0</v>
@@ -40067,7 +40067,7 @@
     </row>
     <row r="404" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
-        <v>432</v>
+        <v>382</v>
       </c>
       <c r="B404">
         <v>0</v>
@@ -40162,7 +40162,7 @@
     </row>
     <row r="405" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
-        <v>433</v>
+        <v>383</v>
       </c>
       <c r="B405">
         <v>0</v>
@@ -40257,7 +40257,7 @@
     </row>
     <row r="406" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
-        <v>434</v>
+        <v>384</v>
       </c>
       <c r="B406">
         <v>17</v>
@@ -40352,7 +40352,7 @@
     </row>
     <row r="407" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
-        <v>435</v>
+        <v>385</v>
       </c>
       <c r="B407">
         <v>0</v>
@@ -40447,7 +40447,7 @@
     </row>
     <row r="408" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
-        <v>436</v>
+        <v>386</v>
       </c>
       <c r="B408">
         <v>0</v>
@@ -40542,7 +40542,7 @@
     </row>
     <row r="409" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
-        <v>437</v>
+        <v>387</v>
       </c>
       <c r="B409">
         <v>4</v>
@@ -40637,7 +40637,7 @@
     </row>
     <row r="410" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
-        <v>438</v>
+        <v>388</v>
       </c>
       <c r="B410">
         <v>1</v>
@@ -40732,7 +40732,7 @@
     </row>
     <row r="411" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
-        <v>439</v>
+        <v>389</v>
       </c>
       <c r="B411">
         <v>0</v>
@@ -40827,7 +40827,7 @@
     </row>
     <row r="412" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
-        <v>440</v>
+        <v>390</v>
       </c>
       <c r="B412">
         <v>0</v>
@@ -40922,7 +40922,7 @@
     </row>
     <row r="413" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
-        <v>441</v>
+        <v>391</v>
       </c>
       <c r="B413">
         <v>0</v>
@@ -41017,7 +41017,7 @@
     </row>
     <row r="414" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
-        <v>442</v>
+        <v>392</v>
       </c>
       <c r="B414">
         <v>0</v>
@@ -41112,7 +41112,7 @@
     </row>
     <row r="415" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
-        <v>443</v>
+        <v>393</v>
       </c>
       <c r="B415">
         <v>0</v>
@@ -41207,7 +41207,7 @@
     </row>
     <row r="416" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
-        <v>444</v>
+        <v>394</v>
       </c>
       <c r="B416">
         <v>0</v>
@@ -41302,7 +41302,7 @@
     </row>
     <row r="417" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
-        <v>445</v>
+        <v>395</v>
       </c>
       <c r="B417">
         <v>0</v>
@@ -41397,7 +41397,7 @@
     </row>
     <row r="418" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
-        <v>446</v>
+        <v>396</v>
       </c>
       <c r="B418">
         <v>0</v>
@@ -41492,7 +41492,7 @@
     </row>
     <row r="419" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
-        <v>447</v>
+        <v>397</v>
       </c>
       <c r="B419">
         <v>0</v>
@@ -41587,7 +41587,7 @@
     </row>
     <row r="420" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
-        <v>448</v>
+        <v>398</v>
       </c>
       <c r="B420">
         <v>0</v>
@@ -41682,7 +41682,7 @@
     </row>
     <row r="421" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
-        <v>449</v>
+        <v>399</v>
       </c>
       <c r="B421">
         <v>0</v>
@@ -41777,7 +41777,7 @@
     </row>
     <row r="422" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
-        <v>450</v>
+        <v>400</v>
       </c>
       <c r="B422">
         <v>0</v>
@@ -41872,7 +41872,7 @@
     </row>
     <row r="423" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
-        <v>451</v>
+        <v>401</v>
       </c>
       <c r="B423">
         <v>0</v>
@@ -41967,7 +41967,7 @@
     </row>
     <row r="424" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
-        <v>452</v>
+        <v>402</v>
       </c>
       <c r="B424">
         <v>0</v>
@@ -42062,7 +42062,7 @@
     </row>
     <row r="425" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A425" t="s">
-        <v>453</v>
+        <v>403</v>
       </c>
       <c r="B425">
         <v>0</v>
@@ -42157,7 +42157,7 @@
     </row>
     <row r="426" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A426" t="s">
-        <v>454</v>
+        <v>404</v>
       </c>
       <c r="B426">
         <v>0</v>
@@ -42252,7 +42252,7 @@
     </row>
     <row r="427" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A427" t="s">
-        <v>455</v>
+        <v>405</v>
       </c>
       <c r="B427">
         <v>0</v>
@@ -42347,7 +42347,7 @@
     </row>
     <row r="428" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A428" t="s">
-        <v>456</v>
+        <v>406</v>
       </c>
       <c r="B428">
         <v>0</v>
@@ -42442,7 +42442,7 @@
     </row>
     <row r="429" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A429" t="s">
-        <v>457</v>
+        <v>407</v>
       </c>
       <c r="B429">
         <v>0</v>
@@ -42537,7 +42537,7 @@
     </row>
     <row r="430" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A430" t="s">
-        <v>458</v>
+        <v>408</v>
       </c>
       <c r="B430">
         <v>0</v>
@@ -42632,7 +42632,7 @@
     </row>
     <row r="431" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A431" t="s">
-        <v>459</v>
+        <v>409</v>
       </c>
       <c r="B431">
         <v>0</v>
@@ -42740,23 +42740,23 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>460</v>
+        <v>410</v>
       </c>
       <c r="B1" t="s">
-        <v>461</v>
+        <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>462</v>
+        <v>412</v>
       </c>
       <c r="B2" t="s">
-        <v>463</v>
+        <v>413</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>464</v>
+        <v>414</v>
       </c>
       <c r="B3">
         <v>820</v>
@@ -42764,7 +42764,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>465</v>
+        <v>415</v>
       </c>
       <c r="B4">
         <v>4054</v>
@@ -42772,10 +42772,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>466</v>
+        <v>416</v>
       </c>
       <c r="B5" t="s">
-        <v>467</v>
+        <v>417</v>
       </c>
     </row>
   </sheetData>

</xml_diff>